<commit_message>
[IMPL] CRUD PLAGAS COMPLETO Se ha implementado la funcionalidad de listar PLAGAS Se ha implementado la funcionalidad de introducir una nueva plaga Se ha implementado la funcionalidad de eliminar una plaga
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E50CF62-60A3-484F-AAA8-EC47802D93AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF739C92-A3D7-4C69-B800-41043D53E8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29145" yWindow="690" windowWidth="20145" windowHeight="9705" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -1649,94 +1649,94 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>34</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3530,8 +3530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -4372,12 +4372,14 @@
       <c r="C41" s="5">
         <v>44257</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="5">
+        <v>44257</v>
+      </c>
       <c r="E41" s="5">
         <v>44259</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -4391,12 +4393,14 @@
       <c r="C42" s="5">
         <v>44257</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5">
+        <v>44257</v>
+      </c>
       <c r="E42" s="5">
         <v>44259</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -4410,12 +4414,14 @@
       <c r="C43" s="5">
         <v>44258</v>
       </c>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5">
+        <v>44257</v>
+      </c>
       <c r="E43" s="5">
         <v>44260</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -4429,12 +4435,14 @@
       <c r="C44" s="5">
         <v>44258</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5">
+        <v>44257</v>
+      </c>
       <c r="E44" s="5">
         <v>44260</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -4448,12 +4456,14 @@
       <c r="C45" s="5">
         <v>44259</v>
       </c>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5">
+        <v>44257</v>
+      </c>
       <c r="E45" s="5">
         <v>44263</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G45" s="1"/>
     </row>
@@ -6636,11 +6646,11 @@
       </c>
       <c r="J12" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K12" s="8">
         <f>K11- J12</f>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -6678,7 +6688,7 @@
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6716,7 +6726,7 @@
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -6754,7 +6764,7 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -6792,7 +6802,7 @@
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -6830,7 +6840,7 @@
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -6868,7 +6878,7 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -6907,7 +6917,7 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -6945,7 +6955,7 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -6983,7 +6993,7 @@
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7021,7 +7031,7 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7059,7 +7069,7 @@
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7097,7 +7107,7 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7135,7 +7145,7 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7173,7 +7183,7 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7211,7 +7221,7 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7249,7 +7259,7 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7287,7 +7297,7 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7325,7 +7335,7 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7363,7 +7373,7 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7401,7 +7411,7 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7439,7 +7449,7 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7477,7 +7487,7 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7515,7 +7525,7 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7553,7 +7563,7 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -7591,7 +7601,7 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -7629,7 +7639,7 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -7649,7 +7659,7 @@
       </c>
       <c r="K39" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -7669,7 +7679,7 @@
       </c>
       <c r="K40" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -7689,7 +7699,7 @@
       </c>
       <c r="K41" s="8">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD TRATAMIENTOS ADMINISTRADOR Se ha implementado el CRUD de tratamientos para el rol administrador. Las funciones implementadas son las siguientes: - Listar los tratamientos - Mostrar detalles de un tratamiento - Editar los detalles de un tratamiento - Eliminar un tratamiento.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF739C92-A3D7-4C69-B800-41043D53E8EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9AFBBE-45ED-4012-8089-4CF54B947C44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="690" windowWidth="20145" windowHeight="9705" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="0" yWindow="1090" windowWidth="20150" windowHeight="9710" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -1652,91 +1652,91 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>29</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3530,8 +3530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -4477,12 +4477,14 @@
       <c r="C46" s="5">
         <v>44259</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5">
+        <v>44258</v>
+      </c>
       <c r="E46" s="5">
         <v>44263</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G46" s="1"/>
     </row>
@@ -4496,12 +4498,14 @@
       <c r="C47" s="5">
         <v>44260</v>
       </c>
-      <c r="D47" s="5"/>
+      <c r="D47" s="5">
+        <v>44258</v>
+      </c>
       <c r="E47" s="5">
         <v>44263</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -4515,12 +4519,14 @@
       <c r="C48" s="5">
         <v>44260</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5">
+        <v>44258</v>
+      </c>
       <c r="E48" s="5">
         <v>44263</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -4534,12 +4540,14 @@
       <c r="C49" s="5">
         <v>44263</v>
       </c>
-      <c r="D49" s="5"/>
+      <c r="D49" s="5">
+        <v>44258</v>
+      </c>
       <c r="E49" s="5">
         <v>44265</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -4553,12 +4561,14 @@
       <c r="C50" s="5">
         <v>44263</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5">
+        <v>44258</v>
+      </c>
       <c r="E50" s="5">
         <v>44265</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -4572,12 +4582,14 @@
       <c r="C51" s="5">
         <v>44264</v>
       </c>
-      <c r="D51" s="5"/>
+      <c r="D51" s="5">
+        <v>44262</v>
+      </c>
       <c r="E51" s="5">
         <v>44266</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -4591,12 +4603,14 @@
       <c r="C52" s="5">
         <v>44264</v>
       </c>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5">
+        <v>44259</v>
+      </c>
       <c r="E52" s="5">
         <v>44266</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -4615,7 +4629,7 @@
         <v>44267</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -6474,8 +6488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6684,11 +6698,11 @@
       </c>
       <c r="J13" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6722,11 +6736,11 @@
       </c>
       <c r="J14" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -6764,7 +6778,7 @@
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -6802,7 +6816,7 @@
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -6836,11 +6850,11 @@
       </c>
       <c r="J17" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -6878,7 +6892,7 @@
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -6917,7 +6931,7 @@
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -6955,7 +6969,7 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -6993,7 +7007,7 @@
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7031,7 +7045,7 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7069,7 +7083,7 @@
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7107,7 +7121,7 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7145,7 +7159,7 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7183,7 +7197,7 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7221,7 +7235,7 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7259,7 +7273,7 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7297,7 +7311,7 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7335,7 +7349,7 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7373,7 +7387,7 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7411,7 +7425,7 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7449,7 +7463,7 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7487,7 +7501,7 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7525,7 +7539,7 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7563,7 +7577,7 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -7601,7 +7615,7 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -7639,7 +7653,7 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -7659,7 +7673,7 @@
       </c>
       <c r="K39" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -7679,7 +7693,7 @@
       </c>
       <c r="K40" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -7699,7 +7713,7 @@
       </c>
       <c r="K41" s="8">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD FACTURAS REALIZADO Se ha implementado el modelo de facturas Se ha implementado la funcionalidad de mostrar facturas para el rol de cliente Se ha implementado la funcionalidad de listar facturas para el rol de administrador Se ha implementado la funcionalidad de mostrar facturas para el rol de administrador
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9AFBBE-45ED-4012-8089-4CF54B947C44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B35847-DB9F-43F9-9773-29A75219F5BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1090" windowWidth="20150" windowHeight="9710" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="28800" yWindow="1170" windowWidth="14340" windowHeight="6900" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 26/03/2021</t>
+  </si>
+  <si>
+    <t>Creación de la vista de árbol  de facturas</t>
+  </si>
+  <si>
+    <t>Creación de la vista de formulario de facturas</t>
   </si>
 </sst>
 </file>
@@ -1667,76 +1673,76 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>22</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3530,8 +3536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -3541,6 +3547,7 @@
     <col min="3" max="3" width="13.1796875" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
@@ -4624,18 +4631,20 @@
       <c r="C53" s="5">
         <v>44265</v>
       </c>
-      <c r="D53" s="5"/>
+      <c r="D53" s="5">
+        <v>44263</v>
+      </c>
       <c r="E53" s="5">
         <v>44267</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B54" s="12">
         <v>1</v>
@@ -4643,18 +4652,20 @@
       <c r="C54" s="5">
         <v>44265</v>
       </c>
-      <c r="D54" s="5"/>
+      <c r="D54" s="5">
+        <v>44264</v>
+      </c>
       <c r="E54" s="5">
         <v>44267</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B55" s="12">
         <v>1</v>
@@ -4662,12 +4673,14 @@
       <c r="C55" s="5">
         <v>44266</v>
       </c>
-      <c r="D55" s="5"/>
+      <c r="D55" s="5">
+        <v>44264</v>
+      </c>
       <c r="E55" s="5">
         <v>44270</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G55" s="1"/>
     </row>
@@ -4681,12 +4694,14 @@
       <c r="C56" s="5">
         <v>44266</v>
       </c>
-      <c r="D56" s="5"/>
+      <c r="D56" s="5">
+        <v>44264</v>
+      </c>
       <c r="E56" s="5">
         <v>44270</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -4700,12 +4715,14 @@
       <c r="C57" s="5">
         <v>44267</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="5">
+        <v>44264</v>
+      </c>
       <c r="E57" s="5">
         <v>44270</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -4719,7 +4736,9 @@
       <c r="C58" s="5">
         <v>44267</v>
       </c>
-      <c r="D58" s="5"/>
+      <c r="D58" s="5">
+        <v>44264</v>
+      </c>
       <c r="E58" s="5">
         <v>44270</v>
       </c>
@@ -4738,12 +4757,14 @@
       <c r="C59" s="5">
         <v>44270</v>
       </c>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5">
+        <v>44264</v>
+      </c>
       <c r="E59" s="5">
         <v>44272</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -6488,8 +6509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6888,11 +6909,11 @@
       </c>
       <c r="J18" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -6927,11 +6948,11 @@
       </c>
       <c r="J19" s="17">
         <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -6969,7 +6990,7 @@
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -7007,7 +7028,7 @@
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7045,7 +7066,7 @@
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7083,7 +7104,7 @@
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7121,7 +7142,7 @@
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7159,7 +7180,7 @@
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7197,7 +7218,7 @@
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7235,7 +7256,7 @@
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7273,7 +7294,7 @@
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7311,7 +7332,7 @@
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7349,7 +7370,7 @@
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7387,7 +7408,7 @@
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7425,7 +7446,7 @@
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7463,7 +7484,7 @@
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7501,7 +7522,7 @@
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7539,7 +7560,7 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7577,7 +7598,7 @@
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -7615,7 +7636,7 @@
       </c>
       <c r="K37" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -7653,7 +7674,7 @@
       </c>
       <c r="K38" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -7673,7 +7694,7 @@
       </c>
       <c r="K39" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -7693,7 +7714,7 @@
       </c>
       <c r="K40" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -7713,7 +7734,7 @@
       </c>
       <c r="K41" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD VEHICULOS Se he implementado las funcionalidades de listar, mostrar, editar y eliminar vehículos para el rol de administrador. Falta implementar la funcionalidad de asignar un vehículo a un trabajador. Para ello, se tiene que implementar primeramente el CRUD de trabajador para el rol de administrador.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B35847-DB9F-43F9-9773-29A75219F5BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB99C32A-4AEC-475E-83F5-A4FF7BBE45BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1170" windowWidth="14340" windowHeight="6900" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -1417,97 +1417,97 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>38.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.599999999999994</c:v>
+                  <c:v>37.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.399999999999991</c:v>
+                  <c:v>35.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.199999999999992</c:v>
+                  <c:v>34.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.999999999999993</c:v>
+                  <c:v>33.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.799999999999994</c:v>
+                  <c:v>31.999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.599999999999994</c:v>
+                  <c:v>30.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.399999999999995</c:v>
+                  <c:v>29.333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.199999999999996</c:v>
+                  <c:v>27.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>26.666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>23.999999999999996</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>22.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21.599999999999998</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.399999999999999</c:v>
+                  <c:v>22.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.2</c:v>
+                  <c:v>21.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.8</c:v>
+                  <c:v>18.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.600000000000001</c:v>
+                  <c:v>17.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.400000000000002</c:v>
+                  <c:v>16.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.200000000000003</c:v>
+                  <c:v>14.66666666666667</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12.000000000000004</c:v>
+                  <c:v>13.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.800000000000004</c:v>
+                  <c:v>12.000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.600000000000005</c:v>
+                  <c:v>10.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.4000000000000057</c:v>
+                  <c:v>9.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.2000000000000055</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.0000000000000053</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.8000000000000052</c:v>
+                  <c:v>5.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.600000000000005</c:v>
+                  <c:v>4.0000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4000000000000048</c:v>
+                  <c:v>2.6666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2000000000000048</c:v>
+                  <c:v>1.3333333333333346</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.8849813083506888E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,31 +1652,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>14</c:v>
@@ -1694,55 +1694,55 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3534,10 +3534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:G237"/>
+  <dimension ref="A1:G238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -4778,12 +4778,14 @@
       <c r="C60" s="5">
         <v>44270</v>
       </c>
-      <c r="D60" s="5"/>
+      <c r="D60" s="5">
+        <v>44265</v>
+      </c>
       <c r="E60" s="5">
         <v>44272</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -4797,12 +4799,14 @@
       <c r="C61" s="5">
         <v>44271</v>
       </c>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5">
+        <v>44265</v>
+      </c>
       <c r="E61" s="5">
         <v>44273</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -4816,12 +4820,14 @@
       <c r="C62" s="5">
         <v>44271</v>
       </c>
-      <c r="D62" s="5"/>
+      <c r="D62" s="5">
+        <v>44265</v>
+      </c>
       <c r="E62" s="5">
         <v>44273</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -4835,12 +4841,14 @@
       <c r="C63" s="5">
         <v>44272</v>
       </c>
-      <c r="D63" s="5"/>
+      <c r="D63" s="5">
+        <v>44270</v>
+      </c>
       <c r="E63" s="5">
         <v>44274</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G63" s="1"/>
     </row>
@@ -4854,12 +4862,14 @@
       <c r="C64" s="5">
         <v>44272</v>
       </c>
-      <c r="D64" s="5"/>
+      <c r="D64" s="5">
+        <v>44265</v>
+      </c>
       <c r="E64" s="5">
         <v>44274</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -4873,12 +4883,14 @@
       <c r="C65" s="5">
         <v>44273</v>
       </c>
-      <c r="D65" s="5"/>
+      <c r="D65" s="5">
+        <v>44270</v>
+      </c>
       <c r="E65" s="5">
         <v>44277</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -4892,12 +4904,14 @@
       <c r="C66" s="5">
         <v>44273</v>
       </c>
-      <c r="D66" s="5"/>
+      <c r="D66" s="5">
+        <v>44271</v>
+      </c>
       <c r="E66" s="5">
         <v>44277</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -4925,7 +4939,7 @@
         <v>71</v>
       </c>
       <c r="B68" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C68" s="5">
         <v>44274</v>
@@ -4939,19 +4953,19 @@
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="12">
         <v>1</v>
       </c>
       <c r="C69" s="5">
-        <v>44277</v>
+        <v>44274</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5">
-        <v>44279</v>
+        <v>44277</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>5</v>
@@ -4960,52 +4974,62 @@
     </row>
     <row r="70" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B70" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C70" s="5">
-        <v>44278</v>
+        <v>44277</v>
       </c>
       <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
-        <v>80</v>
+      <c r="E70" s="5">
+        <v>44279</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B71" s="12">
         <v>2</v>
       </c>
       <c r="C71" s="5">
-        <v>44279</v>
+        <v>44278</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" s="12">
+        <v>2</v>
+      </c>
+      <c r="C72" s="5">
+        <v>44279</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -6472,7 +6496,15 @@
       <c r="F236" s="1"/>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A237" s="1"/>
+      <c r="B237" s="1"/>
       <c r="C237" s="1"/>
+      <c r="D237" s="1"/>
+      <c r="E237" s="1"/>
+      <c r="F237" s="1"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C238" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F37">
@@ -6497,7 +6529,7 @@
           <x14:formula1>
             <xm:f>AUX!$F$3:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F40:F71 F3:F38</xm:sqref>
+          <xm:sqref>F3:F38 F40:F72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6509,8 +6541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6576,8 +6608,8 @@
         <v>43</v>
       </c>
       <c r="I8" s="13">
-        <f>SUM('SPRINT-BACKLOG'!B40:B71)</f>
-        <v>36</v>
+        <f>SUM('SPRINT-BACKLOG'!B40:B72)</f>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.35">
@@ -6639,15 +6671,15 @@
       </c>
       <c r="I11" s="8">
         <f>I8</f>
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J11" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>2</v>
       </c>
       <c r="K11" s="8">
         <f>I8 - J11</f>
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -6677,15 +6709,15 @@
       </c>
       <c r="I12" s="8">
         <f>I11-$I$8/($I$7-1)</f>
-        <v>34.799999999999997</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="J12" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>5</v>
       </c>
       <c r="K12" s="8">
         <f>K11- J12</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -6715,15 +6747,15 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" ref="I13:I41" si="1">I12-$I$8/($I$7-1)</f>
-        <v>33.599999999999994</v>
+        <v>37.333333333333329</v>
       </c>
       <c r="J13" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>5</v>
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6753,15 +6785,15 @@
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
-        <v>32.399999999999991</v>
+        <v>35.999999999999993</v>
       </c>
       <c r="J14" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>1</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -6791,15 +6823,15 @@
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
-        <v>31.199999999999992</v>
+        <v>34.666666666666657</v>
       </c>
       <c r="J15" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -6829,15 +6861,15 @@
       </c>
       <c r="I16" s="8">
         <f t="shared" si="1"/>
-        <v>29.999999999999993</v>
+        <v>33.333333333333321</v>
       </c>
       <c r="J16" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -6867,15 +6899,15 @@
       </c>
       <c r="I17" s="8">
         <f t="shared" si="1"/>
-        <v>28.799999999999994</v>
+        <v>31.999999999999989</v>
       </c>
       <c r="J17" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>1</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -6905,15 +6937,15 @@
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
-        <v>27.599999999999994</v>
+        <v>30.666666666666657</v>
       </c>
       <c r="J18" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>1</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -6944,15 +6976,15 @@
       </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
-        <v>26.399999999999995</v>
+        <v>29.333333333333325</v>
       </c>
       <c r="J19" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>7</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -6982,11 +7014,11 @@
       </c>
       <c r="I20" s="8">
         <f t="shared" si="1"/>
-        <v>25.199999999999996</v>
+        <v>27.999999999999993</v>
       </c>
       <c r="J20" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B72)</f>
+        <v>4</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
@@ -7020,10 +7052,10 @@
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
-        <v>23.999999999999996</v>
+        <v>26.666666666666661</v>
       </c>
       <c r="J21" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K21" s="8">
@@ -7058,10 +7090,10 @@
       </c>
       <c r="I22" s="8">
         <f t="shared" si="1"/>
-        <v>22.799999999999997</v>
+        <v>25.333333333333329</v>
       </c>
       <c r="J22" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K22" s="8">
@@ -7096,10 +7128,10 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="1"/>
-        <v>21.599999999999998</v>
+        <v>23.999999999999996</v>
       </c>
       <c r="J23" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K23" s="8">
@@ -7134,10 +7166,10 @@
       </c>
       <c r="I24" s="8">
         <f t="shared" si="1"/>
-        <v>20.399999999999999</v>
+        <v>22.666666666666664</v>
       </c>
       <c r="J24" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K24" s="8">
@@ -7172,15 +7204,15 @@
       </c>
       <c r="I25" s="8">
         <f t="shared" si="1"/>
-        <v>19.2</v>
+        <v>21.333333333333332</v>
       </c>
       <c r="J25" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B72)</f>
+        <v>2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7210,15 +7242,15 @@
       </c>
       <c r="I26" s="8">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J26" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B71)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B72)</f>
+        <v>1</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7248,15 +7280,15 @@
       </c>
       <c r="I27" s="8">
         <f t="shared" si="1"/>
-        <v>16.8</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="J27" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7286,15 +7318,15 @@
       </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
-        <v>15.600000000000001</v>
+        <v>17.333333333333336</v>
       </c>
       <c r="J28" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7324,15 +7356,15 @@
       </c>
       <c r="I29" s="8">
         <f t="shared" si="1"/>
-        <v>14.400000000000002</v>
+        <v>16.000000000000004</v>
       </c>
       <c r="J29" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7362,15 +7394,15 @@
       </c>
       <c r="I30" s="8">
         <f t="shared" si="1"/>
-        <v>13.200000000000003</v>
+        <v>14.66666666666667</v>
       </c>
       <c r="J30" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7400,15 +7432,15 @@
       </c>
       <c r="I31" s="8">
         <f t="shared" si="1"/>
-        <v>12.000000000000004</v>
+        <v>13.333333333333336</v>
       </c>
       <c r="J31" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7438,15 +7470,15 @@
       </c>
       <c r="I32" s="8">
         <f t="shared" si="1"/>
-        <v>10.800000000000004</v>
+        <v>12.000000000000002</v>
       </c>
       <c r="J32" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7476,15 +7508,15 @@
       </c>
       <c r="I33" s="8">
         <f t="shared" si="1"/>
-        <v>9.600000000000005</v>
+        <v>10.666666666666668</v>
       </c>
       <c r="J33" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7514,15 +7546,15 @@
       </c>
       <c r="I34" s="8">
         <f t="shared" si="1"/>
-        <v>8.4000000000000057</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="J34" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7552,15 +7584,15 @@
       </c>
       <c r="I35" s="8">
         <f t="shared" si="1"/>
-        <v>7.2000000000000055</v>
+        <v>8</v>
       </c>
       <c r="J35" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7590,15 +7622,15 @@
       </c>
       <c r="I36" s="8">
         <f t="shared" si="1"/>
-        <v>6.0000000000000053</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="J36" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -7628,15 +7660,15 @@
       </c>
       <c r="I37" s="8">
         <f t="shared" si="1"/>
-        <v>4.8000000000000052</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="J37" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K37" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -7666,15 +7698,15 @@
       </c>
       <c r="I38" s="8">
         <f t="shared" si="1"/>
-        <v>3.600000000000005</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="J38" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K38" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -7686,15 +7718,15 @@
       </c>
       <c r="I39" s="8">
         <f t="shared" si="1"/>
-        <v>2.4000000000000048</v>
+        <v>2.6666666666666679</v>
       </c>
       <c r="J39" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K39" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -7706,15 +7738,15 @@
       </c>
       <c r="I40" s="8">
         <f t="shared" si="1"/>
-        <v>1.2000000000000048</v>
+        <v>1.3333333333333346</v>
       </c>
       <c r="J40" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K40" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -7726,15 +7758,15 @@
       </c>
       <c r="I41" s="8">
         <f t="shared" si="1"/>
-        <v>4.8849813083506888E-15</v>
+        <v>0</v>
       </c>
       <c r="J41" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D71,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B71)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B72)</f>
         <v>0</v>
       </c>
       <c r="K41" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD TRABAJADORES Se ha implementado la funcionalidad de listrar trabajadores. Se ha implementado la funcionalidad de añadir un nuevo trabajador. Se ha implementado la funcionalidad de mostrar los detalles de un trabajador. Se ha implementado la funcionalidad de editar los detalles de un trabajador. Se ha implementado la funcionalidad de eliminar a un trabajador, siempre y cuando no tenga un servicio asociado.
HAY UN BUG IMPORTANTE CUANDO SE ASIGNA UN VEHICULO A UN TRABAJADOR, YA QUE LA CACHÉ DEL FORMULARIO NO ES BORRADA POR LO TANTO NO MUESTRA LOS VEHICULOS CORRECTAMENTE.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB99C32A-4AEC-475E-83F5-A4FF7BBE45BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780B3FD9-93F5-4A19-A483-B60E4EF705A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -297,13 +297,31 @@
   </si>
   <si>
     <t>Creación de la vista de formulario de facturas</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de listar trabajadores (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de introducir trabajadores (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de mostrar los detalles de un trabajador (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de editar los detalles de un trabajador (ADMIN)</t>
+  </si>
+  <si>
+    <t>LE HACE FALTA BORRAR CACHE PARA QUE FUNCIONE BIEN</t>
+  </si>
+  <si>
+    <t>Implementación de dar de baja a un trabajador (ADMIN)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,8 +371,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0984E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -503,6 +534,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1417,97 +1451,97 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.666666666666664</c:v>
+                  <c:v>43.016666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.333333333333329</c:v>
+                  <c:v>41.533333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.999999999999993</c:v>
+                  <c:v>40.049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.666666666666657</c:v>
+                  <c:v>38.566666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.333333333333321</c:v>
+                  <c:v>37.083333333333329</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.999999999999989</c:v>
+                  <c:v>35.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.666666666666657</c:v>
+                  <c:v>34.11666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.333333333333325</c:v>
+                  <c:v>32.633333333333326</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.999999999999993</c:v>
+                  <c:v>31.149999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.666666666666661</c:v>
+                  <c:v>29.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.333333333333329</c:v>
+                  <c:v>28.183333333333323</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.999999999999996</c:v>
+                  <c:v>26.699999999999989</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.666666666666664</c:v>
+                  <c:v>25.216666666666654</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.333333333333332</c:v>
+                  <c:v>23.73333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>22.249999999999986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.666666666666668</c:v>
+                  <c:v>20.766666666666652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.333333333333336</c:v>
+                  <c:v>19.283333333333317</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.000000000000004</c:v>
+                  <c:v>17.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.66666666666667</c:v>
+                  <c:v>16.316666666666649</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.333333333333336</c:v>
+                  <c:v>14.833333333333314</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.000000000000002</c:v>
+                  <c:v>13.34999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.666666666666668</c:v>
+                  <c:v>11.866666666666646</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.3333333333333339</c:v>
+                  <c:v>10.383333333333312</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8</c:v>
+                  <c:v>8.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>7.4166666666666439</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.3333333333333339</c:v>
+                  <c:v>5.9333333333333105</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0000000000000009</c:v>
+                  <c:v>4.4499999999999771</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.6666666666666679</c:v>
+                  <c:v>2.9666666666666437</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3333333333333346</c:v>
+                  <c:v>1.4833333333333103</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>-2.3092638912203256E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1652,97 +1686,97 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3198,16 +3232,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>758825</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>20492</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>50511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>578304</xdr:colOff>
+      <xdr:colOff>595621</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>399144</xdr:rowOff>
+      <xdr:rowOff>436955</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3534,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:G238"/>
+  <dimension ref="A1:H243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -4873,7 +4907,7 @@
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>68</v>
       </c>
@@ -4894,7 +4928,7 @@
       </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
@@ -4915,47 +4949,43 @@
       </c>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B67" s="12">
         <v>1</v>
       </c>
-      <c r="C67" s="5">
-        <v>44274</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5">
-        <v>44277</v>
-      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5">
+        <v>44271</v>
+      </c>
+      <c r="E67" s="5"/>
       <c r="F67" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B68" s="12">
-        <v>4</v>
-      </c>
-      <c r="C68" s="5">
-        <v>44274</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5">
-        <v>44277</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5">
+        <v>44272</v>
+      </c>
+      <c r="E68" s="5"/>
       <c r="F68" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B69" s="12">
         <v>1</v>
@@ -4963,121 +4993,174 @@
       <c r="C69" s="5">
         <v>44274</v>
       </c>
-      <c r="D69" s="5"/>
+      <c r="D69" s="5">
+        <v>44271</v>
+      </c>
       <c r="E69" s="5">
         <v>44277</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B70" s="12">
         <v>1</v>
       </c>
       <c r="C70" s="5">
+        <v>44276</v>
+      </c>
+      <c r="D70" s="5">
+        <v>44271</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="12">
+        <v>1</v>
+      </c>
+      <c r="C71" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D71" s="5">
+        <v>44276</v>
+      </c>
+      <c r="E71" s="5">
         <v>44277</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5">
+      <c r="F71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="H71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5">
+        <v>44276</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="12">
+        <v>4</v>
+      </c>
+      <c r="C73" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5">
+        <v>44277</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1</v>
+      </c>
+      <c r="C74" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5">
+        <v>44277</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="12">
+        <v>1</v>
+      </c>
+      <c r="C75" s="5">
+        <v>44277</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5">
         <v>44279</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.5" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B71" s="12">
+      <c r="B76" s="12">
         <v>2</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C76" s="5">
         <v>44278</v>
       </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B72" s="12">
+      <c r="B77" s="12">
         <v>2</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C77" s="5">
         <v>44279</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="s">
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F77" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -5086,7 +5169,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -6504,7 +6587,47 @@
       <c r="F237" s="1"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
       <c r="C238" s="1"/>
+      <c r="D238" s="1"/>
+      <c r="E238" s="1"/>
+      <c r="F238" s="1"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1"/>
+      <c r="E239" s="1"/>
+      <c r="F239" s="1"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="1"/>
+      <c r="E240" s="1"/>
+      <c r="F240" s="1"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1"/>
+      <c r="E241" s="1"/>
+      <c r="F241" s="1"/>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="1"/>
+      <c r="E242" s="1"/>
+      <c r="F242" s="1"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C243" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F37">
@@ -6529,7 +6652,7 @@
           <x14:formula1>
             <xm:f>AUX!$F$3:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F38 F40:F72</xm:sqref>
+          <xm:sqref>F3:F38 F40:F77</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6541,8 +6664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6608,8 +6731,8 @@
         <v>43</v>
       </c>
       <c r="I8" s="13">
-        <f>SUM('SPRINT-BACKLOG'!B40:B72)</f>
-        <v>40</v>
+        <f>SUM('SPRINT-BACKLOG'!B40:B77)</f>
+        <v>44.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.35">
@@ -6671,15 +6794,15 @@
       </c>
       <c r="I11" s="8">
         <f>I8</f>
-        <v>40</v>
+        <v>44.5</v>
       </c>
       <c r="J11" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>2</v>
       </c>
       <c r="K11" s="8">
         <f>I8 - J11</f>
-        <v>38</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -6709,15 +6832,15 @@
       </c>
       <c r="I12" s="8">
         <f>I11-$I$8/($I$7-1)</f>
-        <v>38.666666666666664</v>
+        <v>43.016666666666666</v>
       </c>
       <c r="J12" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>5</v>
       </c>
       <c r="K12" s="8">
         <f>K11- J12</f>
-        <v>33</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -6747,15 +6870,15 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" ref="I13:I41" si="1">I12-$I$8/($I$7-1)</f>
-        <v>37.333333333333329</v>
+        <v>41.533333333333331</v>
       </c>
       <c r="J13" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>5</v>
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>28</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6785,15 +6908,15 @@
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
-        <v>35.999999999999993</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="J14" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>1</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>27</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -6823,15 +6946,15 @@
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
-        <v>34.666666666666657</v>
+        <v>38.566666666666663</v>
       </c>
       <c r="J15" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -6861,15 +6984,15 @@
       </c>
       <c r="I16" s="8">
         <f t="shared" si="1"/>
-        <v>33.333333333333321</v>
+        <v>37.083333333333329</v>
       </c>
       <c r="J16" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -6899,15 +7022,15 @@
       </c>
       <c r="I17" s="8">
         <f t="shared" si="1"/>
-        <v>31.999999999999989</v>
+        <v>35.599999999999994</v>
       </c>
       <c r="J17" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>1</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -6937,15 +7060,15 @@
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
-        <v>30.666666666666657</v>
+        <v>34.11666666666666</v>
       </c>
       <c r="J18" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>1</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -6976,15 +7099,15 @@
       </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
-        <v>29.333333333333325</v>
+        <v>32.633333333333326</v>
       </c>
       <c r="J19" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>7</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -7014,15 +7137,15 @@
       </c>
       <c r="I20" s="8">
         <f t="shared" si="1"/>
-        <v>27.999999999999993</v>
+        <v>31.149999999999991</v>
       </c>
       <c r="J20" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>4</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -7052,15 +7175,15 @@
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
-        <v>26.666666666666661</v>
+        <v>29.666666666666657</v>
       </c>
       <c r="J21" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7090,15 +7213,15 @@
       </c>
       <c r="I22" s="8">
         <f t="shared" si="1"/>
-        <v>25.333333333333329</v>
+        <v>28.183333333333323</v>
       </c>
       <c r="J22" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7128,15 +7251,15 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="1"/>
-        <v>23.999999999999996</v>
+        <v>26.699999999999989</v>
       </c>
       <c r="J23" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7166,15 +7289,15 @@
       </c>
       <c r="I24" s="8">
         <f t="shared" si="1"/>
-        <v>22.666666666666664</v>
+        <v>25.216666666666654</v>
       </c>
       <c r="J24" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7204,15 +7327,15 @@
       </c>
       <c r="I25" s="8">
         <f t="shared" si="1"/>
-        <v>21.333333333333332</v>
+        <v>23.73333333333332</v>
       </c>
       <c r="J25" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7242,15 +7365,15 @@
       </c>
       <c r="I26" s="8">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>22.249999999999986</v>
       </c>
       <c r="J26" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B72)</f>
-        <v>1</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B77)</f>
+        <v>4</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7280,15 +7403,15 @@
       </c>
       <c r="I27" s="8">
         <f t="shared" si="1"/>
-        <v>18.666666666666668</v>
+        <v>20.766666666666652</v>
       </c>
       <c r="J27" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B72)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B77)</f>
+        <v>1</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7318,15 +7441,15 @@
       </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
-        <v>17.333333333333336</v>
+        <v>19.283333333333317</v>
       </c>
       <c r="J28" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7356,15 +7479,15 @@
       </c>
       <c r="I29" s="8">
         <f t="shared" si="1"/>
-        <v>16.000000000000004</v>
+        <v>17.799999999999983</v>
       </c>
       <c r="J29" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7394,15 +7517,15 @@
       </c>
       <c r="I30" s="8">
         <f t="shared" si="1"/>
-        <v>14.66666666666667</v>
+        <v>16.316666666666649</v>
       </c>
       <c r="J30" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7432,15 +7555,15 @@
       </c>
       <c r="I31" s="8">
         <f t="shared" si="1"/>
-        <v>13.333333333333336</v>
+        <v>14.833333333333314</v>
       </c>
       <c r="J31" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B72)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B77)</f>
+        <v>1.5</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7470,15 +7593,15 @@
       </c>
       <c r="I32" s="8">
         <f t="shared" si="1"/>
-        <v>12.000000000000002</v>
+        <v>13.34999999999998</v>
       </c>
       <c r="J32" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7508,15 +7631,15 @@
       </c>
       <c r="I33" s="8">
         <f t="shared" si="1"/>
-        <v>10.666666666666668</v>
+        <v>11.866666666666646</v>
       </c>
       <c r="J33" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7546,15 +7669,15 @@
       </c>
       <c r="I34" s="8">
         <f t="shared" si="1"/>
-        <v>9.3333333333333339</v>
+        <v>10.383333333333312</v>
       </c>
       <c r="J34" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7584,15 +7707,15 @@
       </c>
       <c r="I35" s="8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>8.8999999999999773</v>
       </c>
       <c r="J35" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7622,15 +7745,15 @@
       </c>
       <c r="I36" s="8">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
+        <v>7.4166666666666439</v>
       </c>
       <c r="J36" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -7660,15 +7783,15 @@
       </c>
       <c r="I37" s="8">
         <f t="shared" si="1"/>
-        <v>5.3333333333333339</v>
+        <v>5.9333333333333105</v>
       </c>
       <c r="J37" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K37" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -7698,15 +7821,15 @@
       </c>
       <c r="I38" s="8">
         <f t="shared" si="1"/>
-        <v>4.0000000000000009</v>
+        <v>4.4499999999999771</v>
       </c>
       <c r="J38" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K38" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -7718,15 +7841,15 @@
       </c>
       <c r="I39" s="8">
         <f t="shared" si="1"/>
-        <v>2.6666666666666679</v>
+        <v>2.9666666666666437</v>
       </c>
       <c r="J39" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K39" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -7738,15 +7861,15 @@
       </c>
       <c r="I40" s="8">
         <f t="shared" si="1"/>
-        <v>1.3333333333333346</v>
+        <v>1.4833333333333103</v>
       </c>
       <c r="J40" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K40" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -7758,15 +7881,15 @@
       </c>
       <c r="I41" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.3092638912203256E-14</v>
       </c>
       <c r="J41" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D72,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B72)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B77)</f>
         <v>0</v>
       </c>
       <c r="K41" s="8">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMPL] CRUD TRABAJADOR/EMPRESA (ADMIN) Se ha implementado la funcionalidad de listar los clientes que están dados de alta en la aplicación. Se ha implementado la funcionalidad de mostrar los detalles de un cliente. Se ha implementado la funcionalidad de listar las empresas que están dados de alta en la aplicación. Se ha implementado la funcionalidad de mostrar los detalles de un empresas.
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780B3FD9-93F5-4A19-A483-B60E4EF705A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14840A06-BCDC-45A9-B67F-5EFC7D876FB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>Implementación de dar de baja a un trabajador (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de listar un cliente (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de mostrar los detalles de un cliente (ADMIN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementación de la funcionalidad de listar una empresa (ADMIN) </t>
+  </si>
+  <si>
+    <t>Implementación de mostrar los detalles de una empresa (ADMIN)</t>
   </si>
 </sst>
 </file>
@@ -520,6 +532,9 @@
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -534,9 +549,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,97 +1463,97 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>44.5</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.016666666666666</c:v>
+                  <c:v>46.883333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.533333333333331</c:v>
+                  <c:v>45.266666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.049999999999997</c:v>
+                  <c:v>43.65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.566666666666663</c:v>
+                  <c:v>42.033333333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.083333333333329</c:v>
+                  <c:v>40.416666666666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.599999999999994</c:v>
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.11666666666666</c:v>
+                  <c:v>37.18333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.633333333333326</c:v>
+                  <c:v>35.566666666666663</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.149999999999991</c:v>
+                  <c:v>33.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.666666666666657</c:v>
+                  <c:v>32.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.183333333333323</c:v>
+                  <c:v>30.716666666666661</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.699999999999989</c:v>
+                  <c:v>29.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.216666666666654</c:v>
+                  <c:v>27.483333333333327</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.73333333333332</c:v>
+                  <c:v>25.86666666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.249999999999986</c:v>
+                  <c:v>24.249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.766666666666652</c:v>
+                  <c:v>22.633333333333326</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.283333333333317</c:v>
+                  <c:v>21.016666666666659</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.799999999999983</c:v>
+                  <c:v>19.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16.316666666666649</c:v>
+                  <c:v>17.783333333333324</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.833333333333314</c:v>
+                  <c:v>16.166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.34999999999998</c:v>
+                  <c:v>14.54999999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.866666666666646</c:v>
+                  <c:v>12.933333333333323</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.383333333333312</c:v>
+                  <c:v>11.316666666666656</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.8999999999999773</c:v>
+                  <c:v>9.6999999999999886</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4166666666666439</c:v>
+                  <c:v>8.0833333333333215</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.9333333333333105</c:v>
+                  <c:v>6.4666666666666544</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.4499999999999771</c:v>
+                  <c:v>4.8499999999999872</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.9666666666666437</c:v>
+                  <c:v>3.2333333333333205</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.4833333333333103</c:v>
+                  <c:v>1.6166666666666538</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-2.3092638912203256E-14</c:v>
+                  <c:v>-1.2878587085651816E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,67 +1698,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>42.5</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.5</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.5</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.5</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>22.5</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>18.5</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>16.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>12.5</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>10</c:v>
@@ -3568,10 +3580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:H243"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -3605,14 +3617,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
@@ -4372,14 +4384,14 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="15.5" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" ht="31" outlineLevel="1" x14ac:dyDescent="0.35">
@@ -5042,7 +5054,7 @@
       <c r="F71" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G71" s="23"/>
+      <c r="G71" s="18"/>
       <c r="H71" t="s">
         <v>91</v>
       </c>
@@ -5064,26 +5076,24 @@
     </row>
     <row r="73" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B73" s="12">
-        <v>4</v>
-      </c>
-      <c r="C73" s="5">
-        <v>44274</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5">
+        <v>1</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5">
         <v>44277</v>
       </c>
+      <c r="E73" s="5"/>
       <c r="F73" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B74" s="12">
         <v>1</v>
@@ -5091,109 +5101,151 @@
       <c r="C74" s="5">
         <v>44274</v>
       </c>
-      <c r="D74" s="5"/>
+      <c r="D74" s="5">
+        <v>44277</v>
+      </c>
       <c r="E74" s="5">
         <v>44277</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B75" s="12">
         <v>1</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5">
         <v>44277</v>
       </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5">
-        <v>44279</v>
-      </c>
+      <c r="E75" s="5"/>
       <c r="F75" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="B76" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="5">
-        <v>44278</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
-        <v>80</v>
+        <v>44274</v>
+      </c>
+      <c r="D76" s="5">
+        <v>44277</v>
+      </c>
+      <c r="E76" s="5">
+        <v>44277</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B77" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C77" s="5">
-        <v>44279</v>
+        <v>44274</v>
       </c>
       <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>82</v>
+      <c r="E77" s="5">
+        <v>44277</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" s="12">
+        <v>1</v>
+      </c>
+      <c r="C78" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5">
+        <v>44277</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+    <row r="79" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79" s="12">
+        <v>1</v>
+      </c>
+      <c r="C79" s="5">
+        <v>44277</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5">
+        <v>44279</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
+    <row r="80" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" s="12">
+        <v>2</v>
+      </c>
+      <c r="C80" s="5">
+        <v>44278</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="12">
+        <v>2</v>
+      </c>
+      <c r="C81" s="5">
+        <v>44279</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -6627,7 +6679,39 @@
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
       <c r="C243" s="1"/>
+      <c r="D243" s="1"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="1"/>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="1"/>
+      <c r="E244" s="1"/>
+      <c r="F244" s="1"/>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1"/>
+      <c r="E245" s="1"/>
+      <c r="F245" s="1"/>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1"/>
+      <c r="E246" s="1"/>
+      <c r="F246" s="1"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C247" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F37">
@@ -6652,7 +6736,7 @@
           <x14:formula1>
             <xm:f>AUX!$F$3:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F38 F40:F77</xm:sqref>
+          <xm:sqref>F3:F38 F40:F81</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6664,8 +6748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6678,11 +6762,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F3" s="16" t="s">
@@ -6696,14 +6780,14 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="C6" s="22"/>
+      <c r="H6" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -6731,8 +6815,8 @@
         <v>43</v>
       </c>
       <c r="I8" s="13">
-        <f>SUM('SPRINT-BACKLOG'!B40:B77)</f>
-        <v>44.5</v>
+        <f>SUM('SPRINT-BACKLOG'!B40:B81)</f>
+        <v>48.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.35">
@@ -6794,15 +6878,15 @@
       </c>
       <c r="I11" s="8">
         <f>I8</f>
-        <v>44.5</v>
+        <v>48.5</v>
       </c>
       <c r="J11" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>2</v>
       </c>
       <c r="K11" s="8">
         <f>I8 - J11</f>
-        <v>42.5</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -6832,15 +6916,15 @@
       </c>
       <c r="I12" s="8">
         <f>I11-$I$8/($I$7-1)</f>
-        <v>43.016666666666666</v>
+        <v>46.883333333333333</v>
       </c>
       <c r="J12" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>5</v>
       </c>
       <c r="K12" s="8">
         <f>K11- J12</f>
-        <v>37.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -6870,15 +6954,15 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" ref="I13:I41" si="1">I12-$I$8/($I$7-1)</f>
-        <v>41.533333333333331</v>
+        <v>45.266666666666666</v>
       </c>
       <c r="J13" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>5</v>
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6908,15 +6992,15 @@
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
-        <v>40.049999999999997</v>
+        <v>43.65</v>
       </c>
       <c r="J14" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>1</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>31.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -6946,15 +7030,15 @@
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
-        <v>38.566666666666663</v>
+        <v>42.033333333333331</v>
       </c>
       <c r="J15" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>31.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -6984,15 +7068,15 @@
       </c>
       <c r="I16" s="8">
         <f t="shared" si="1"/>
-        <v>37.083333333333329</v>
+        <v>40.416666666666664</v>
       </c>
       <c r="J16" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>31.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -7022,15 +7106,15 @@
       </c>
       <c r="I17" s="8">
         <f t="shared" si="1"/>
-        <v>35.599999999999994</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="J17" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>1</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>30.5</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -7060,15 +7144,15 @@
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
-        <v>34.11666666666666</v>
+        <v>37.18333333333333</v>
       </c>
       <c r="J18" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>1</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>29.5</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -7099,15 +7183,15 @@
       </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
-        <v>32.633333333333326</v>
+        <v>35.566666666666663</v>
       </c>
       <c r="J19" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>7</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -7137,15 +7221,15 @@
       </c>
       <c r="I20" s="8">
         <f t="shared" si="1"/>
-        <v>31.149999999999991</v>
+        <v>33.949999999999996</v>
       </c>
       <c r="J20" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>4</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -7175,15 +7259,15 @@
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
-        <v>29.666666666666657</v>
+        <v>32.333333333333329</v>
       </c>
       <c r="J21" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7213,15 +7297,15 @@
       </c>
       <c r="I22" s="8">
         <f t="shared" si="1"/>
-        <v>28.183333333333323</v>
+        <v>30.716666666666661</v>
       </c>
       <c r="J22" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7251,15 +7335,15 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="1"/>
-        <v>26.699999999999989</v>
+        <v>29.099999999999994</v>
       </c>
       <c r="J23" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7289,15 +7373,15 @@
       </c>
       <c r="I24" s="8">
         <f t="shared" si="1"/>
-        <v>25.216666666666654</v>
+        <v>27.483333333333327</v>
       </c>
       <c r="J24" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7327,15 +7411,15 @@
       </c>
       <c r="I25" s="8">
         <f t="shared" si="1"/>
-        <v>23.73333333333332</v>
+        <v>25.86666666666666</v>
       </c>
       <c r="J25" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>16.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7365,15 +7449,15 @@
       </c>
       <c r="I26" s="8">
         <f t="shared" si="1"/>
-        <v>22.249999999999986</v>
+        <v>24.249999999999993</v>
       </c>
       <c r="J26" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>4</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7403,15 +7487,15 @@
       </c>
       <c r="I27" s="8">
         <f t="shared" si="1"/>
-        <v>20.766666666666652</v>
+        <v>22.633333333333326</v>
       </c>
       <c r="J27" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>1</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7441,15 +7525,15 @@
       </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
-        <v>19.283333333333317</v>
+        <v>21.016666666666659</v>
       </c>
       <c r="J28" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7479,15 +7563,15 @@
       </c>
       <c r="I29" s="8">
         <f t="shared" si="1"/>
-        <v>17.799999999999983</v>
+        <v>19.399999999999991</v>
       </c>
       <c r="J29" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7517,15 +7601,15 @@
       </c>
       <c r="I30" s="8">
         <f t="shared" si="1"/>
-        <v>16.316666666666649</v>
+        <v>17.783333333333324</v>
       </c>
       <c r="J30" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7555,15 +7639,15 @@
       </c>
       <c r="I31" s="8">
         <f t="shared" si="1"/>
-        <v>14.833333333333314</v>
+        <v>16.166666666666657</v>
       </c>
       <c r="J31" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>1.5</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7593,11 +7677,11 @@
       </c>
       <c r="I32" s="8">
         <f t="shared" si="1"/>
-        <v>13.34999999999998</v>
+        <v>14.54999999999999</v>
       </c>
       <c r="J32" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B77)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B81)</f>
+        <v>4</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
@@ -7631,10 +7715,10 @@
       </c>
       <c r="I33" s="8">
         <f t="shared" si="1"/>
-        <v>11.866666666666646</v>
+        <v>12.933333333333323</v>
       </c>
       <c r="J33" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K33" s="8">
@@ -7669,10 +7753,10 @@
       </c>
       <c r="I34" s="8">
         <f t="shared" si="1"/>
-        <v>10.383333333333312</v>
+        <v>11.316666666666656</v>
       </c>
       <c r="J34" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K34" s="8">
@@ -7707,10 +7791,10 @@
       </c>
       <c r="I35" s="8">
         <f t="shared" si="1"/>
-        <v>8.8999999999999773</v>
+        <v>9.6999999999999886</v>
       </c>
       <c r="J35" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K35" s="8">
@@ -7745,10 +7829,10 @@
       </c>
       <c r="I36" s="8">
         <f t="shared" si="1"/>
-        <v>7.4166666666666439</v>
+        <v>8.0833333333333215</v>
       </c>
       <c r="J36" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K36" s="8">
@@ -7783,10 +7867,10 @@
       </c>
       <c r="I37" s="8">
         <f t="shared" si="1"/>
-        <v>5.9333333333333105</v>
+        <v>6.4666666666666544</v>
       </c>
       <c r="J37" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K37" s="8">
@@ -7821,10 +7905,10 @@
       </c>
       <c r="I38" s="8">
         <f t="shared" si="1"/>
-        <v>4.4499999999999771</v>
+        <v>4.8499999999999872</v>
       </c>
       <c r="J38" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K38" s="8">
@@ -7841,10 +7925,10 @@
       </c>
       <c r="I39" s="8">
         <f t="shared" si="1"/>
-        <v>2.9666666666666437</v>
+        <v>3.2333333333333205</v>
       </c>
       <c r="J39" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K39" s="8">
@@ -7861,10 +7945,10 @@
       </c>
       <c r="I40" s="8">
         <f t="shared" si="1"/>
-        <v>1.4833333333333103</v>
+        <v>1.6166666666666538</v>
       </c>
       <c r="J40" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K40" s="8">
@@ -7881,10 +7965,10 @@
       </c>
       <c r="I41" s="8">
         <f t="shared" si="1"/>
-        <v>-2.3092638912203256E-14</v>
+        <v>-1.2878587085651816E-14</v>
       </c>
       <c r="J41" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D77,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B77)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B81)</f>
         <v>0</v>
       </c>
       <c r="K41" s="8">

</xml_diff>

<commit_message>
[IMPL] CRUD ADMINISTRADOR (ADMIN) Se ha implementado las siguientes funcionalidades:     - Listar los administradores     - Mostrar los detalles de un administrador     - Insertar un nuevo adminisitrador     - Modificar los detalles de un administrador     - Eliminar un administrador
POR EL MOMENTO, SE HA ACABADO LA IMPLEMETNACIÓN DE CRUD.
FALTA COMPROBAR QUE FUNCIONA TODO CORRECTAMENTE
</commit_message>
<xml_diff>
--- a/documentación/Product Backlog/Product-Backlog.xlsx
+++ b/documentación/Product Backlog/Product-Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alesk\Desktop\Universidad\TFG_app\TFG_app\documentación\Product Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14840A06-BCDC-45A9-B67F-5EFC7D876FB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D4F40-A253-4698-AA0D-E999206F9E1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
+    <workbookView xWindow="28635" yWindow="4545" windowWidth="20820" windowHeight="11850" xr2:uid="{41FE112A-4516-4423-9CD7-320A9C032A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT-BACKLOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>Puntos de historia</t>
   </si>
@@ -327,6 +327,21 @@
   </si>
   <si>
     <t>Implementación de mostrar los detalles de una empresa (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de mostrar los detalles de un administrador (ADMIN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementación de la funcionalidad de editar los detalles de un administrador(ADMIN) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementación de la funcionalidad de insertar un nuevo administrador (ADMIN) </t>
+  </si>
+  <si>
+    <t>AImplementación de la funcionalidad de listar administradores (ADMIN)</t>
+  </si>
+  <si>
+    <t>Implementación de la funcionalidad de eliminar un administrador (ADMIN)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +595,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1246,7 +1261,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1463,97 +1478,97 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>48.5</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.883333333333333</c:v>
+                  <c:v>51.716666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.266666666666666</c:v>
+                  <c:v>49.933333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.65</c:v>
+                  <c:v>48.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.033333333333331</c:v>
+                  <c:v>46.366666666666674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.416666666666664</c:v>
+                  <c:v>44.583333333333343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.799999999999997</c:v>
+                  <c:v>42.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.18333333333333</c:v>
+                  <c:v>41.01666666666668</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.566666666666663</c:v>
+                  <c:v>39.233333333333348</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.949999999999996</c:v>
+                  <c:v>37.450000000000017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.333333333333329</c:v>
+                  <c:v>35.666666666666686</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.716666666666661</c:v>
+                  <c:v>33.883333333333354</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.099999999999994</c:v>
+                  <c:v>32.100000000000023</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.483333333333327</c:v>
+                  <c:v>30.316666666666688</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.86666666666666</c:v>
+                  <c:v>28.533333333333353</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.249999999999993</c:v>
+                  <c:v>26.750000000000018</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.633333333333326</c:v>
+                  <c:v>24.966666666666683</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.016666666666659</c:v>
+                  <c:v>23.183333333333348</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.399999999999991</c:v>
+                  <c:v>21.400000000000013</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.783333333333324</c:v>
+                  <c:v>19.616666666666678</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.166666666666657</c:v>
+                  <c:v>17.833333333333343</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.54999999999999</c:v>
+                  <c:v>16.050000000000008</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.933333333333323</c:v>
+                  <c:v>14.266666666666675</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.316666666666656</c:v>
+                  <c:v>12.483333333333341</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.6999999999999886</c:v>
+                  <c:v>10.700000000000008</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.0833333333333215</c:v>
+                  <c:v>8.916666666666675</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.4666666666666544</c:v>
+                  <c:v>7.1333333333333417</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.8499999999999872</c:v>
+                  <c:v>5.3500000000000085</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.2333333333333205</c:v>
+                  <c:v>3.5666666666666753</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.6166666666666538</c:v>
+                  <c:v>1.7833333333333419</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.2878587085651816E-14</c:v>
+                  <c:v>8.4376949871511897E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,79 +1713,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>46.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>41.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>36.5</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.5</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>20.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15.5</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>10</c:v>
@@ -3284,7 +3299,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3580,13 +3595,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB024A1-16E4-467A-A83B-A5E93171F59F}">
-  <dimension ref="A1:H247"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:F39"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.90625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -4877,7 +4892,7 @@
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" ht="46.5" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="62" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>66</v>
       </c>
@@ -5152,26 +5167,24 @@
     </row>
     <row r="77" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="B77" s="12">
-        <v>4</v>
-      </c>
-      <c r="C77" s="5">
-        <v>44274</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5">
-        <v>44277</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5">
+        <v>44281</v>
+      </c>
+      <c r="E77" s="5"/>
       <c r="F77" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B78" s="12">
         <v>1</v>
@@ -5179,118 +5192,168 @@
       <c r="C78" s="5">
         <v>44274</v>
       </c>
-      <c r="D78" s="5"/>
+      <c r="D78" s="5">
+        <v>44281</v>
+      </c>
       <c r="E78" s="5">
         <v>44277</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="62" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B79" s="12">
         <v>1</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="5"/>
+      <c r="D79" s="5">
+        <v>44281</v>
+      </c>
+      <c r="E79" s="5"/>
+      <c r="F79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="12">
+        <v>1</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5">
+        <v>44281</v>
+      </c>
+      <c r="E80" s="5"/>
+      <c r="F80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" s="12">
+        <v>1</v>
+      </c>
+      <c r="C81" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D81" s="5">
+        <v>44281</v>
+      </c>
+      <c r="E81" s="5">
         <v>44277</v>
       </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5">
+      <c r="F81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="12">
+        <v>4</v>
+      </c>
+      <c r="C82" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5">
+        <v>44277</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" s="12">
+        <v>1</v>
+      </c>
+      <c r="C83" s="5">
+        <v>44274</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5">
+        <v>44277</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B84" s="12">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5">
+        <v>44277</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5">
         <v>44279</v>
       </c>
-      <c r="F79" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="s">
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="12">
+      <c r="B85" s="12">
         <v>2</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C85" s="5">
         <v>44278</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F80" s="4" t="s">
+      <c r="F85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="s">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="12">
+      <c r="B86" s="12">
         <v>2</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C86" s="5">
         <v>44279</v>
       </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="s">
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="F86" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -6711,7 +6774,47 @@
       <c r="F246" s="1"/>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
       <c r="C247" s="1"/>
+      <c r="D247" s="1"/>
+      <c r="E247" s="1"/>
+      <c r="F247" s="1"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
+      <c r="E248" s="1"/>
+      <c r="F248" s="1"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="1"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="1"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="1"/>
+      <c r="E250" s="1"/>
+      <c r="F250" s="1"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="1"/>
+      <c r="E251" s="1"/>
+      <c r="F251" s="1"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C252" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F37">
@@ -6736,7 +6839,7 @@
           <x14:formula1>
             <xm:f>AUX!$F$3:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F38 F40:F81</xm:sqref>
+          <xm:sqref>F3:F38 F40:F86</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6748,11 +6851,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ACDF49-AC43-4CCD-856F-6ED289E70C3E}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
@@ -6815,8 +6918,8 @@
         <v>43</v>
       </c>
       <c r="I8" s="13">
-        <f>SUM('SPRINT-BACKLOG'!B40:B81)</f>
-        <v>48.5</v>
+        <f>SUM('SPRINT-BACKLOG'!B40:B86)</f>
+        <v>53.5</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.35">
@@ -6878,15 +6981,15 @@
       </c>
       <c r="I11" s="8">
         <f>I8</f>
-        <v>48.5</v>
+        <v>53.5</v>
       </c>
       <c r="J11" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G11),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>2</v>
       </c>
       <c r="K11" s="8">
         <f>I8 - J11</f>
-        <v>46.5</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -6916,15 +7019,15 @@
       </c>
       <c r="I12" s="8">
         <f>I11-$I$8/($I$7-1)</f>
-        <v>46.883333333333333</v>
+        <v>51.716666666666669</v>
       </c>
       <c r="J12" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G12),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>5</v>
       </c>
       <c r="K12" s="8">
         <f>K11- J12</f>
-        <v>41.5</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -6954,15 +7057,15 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" ref="I13:I41" si="1">I12-$I$8/($I$7-1)</f>
-        <v>45.266666666666666</v>
+        <v>49.933333333333337</v>
       </c>
       <c r="J13" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G13),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>5</v>
       </c>
       <c r="K13" s="8">
         <f>K12- J13</f>
-        <v>36.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -6992,15 +7095,15 @@
       </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
-        <v>43.65</v>
+        <v>48.150000000000006</v>
       </c>
       <c r="J14" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G14),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>1</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" ref="K14:K41" si="3">K13- J14</f>
-        <v>35.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -7030,15 +7133,15 @@
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
-        <v>42.033333333333331</v>
+        <v>46.366666666666674</v>
       </c>
       <c r="J15" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G15),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" si="3"/>
-        <v>35.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -7068,15 +7171,15 @@
       </c>
       <c r="I16" s="8">
         <f t="shared" si="1"/>
-        <v>40.416666666666664</v>
+        <v>44.583333333333343</v>
       </c>
       <c r="J16" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G16),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="3"/>
-        <v>35.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -7106,15 +7209,15 @@
       </c>
       <c r="I17" s="8">
         <f t="shared" si="1"/>
-        <v>38.799999999999997</v>
+        <v>42.800000000000011</v>
       </c>
       <c r="J17" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G17),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>1</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="3"/>
-        <v>34.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -7144,15 +7247,15 @@
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
-        <v>37.18333333333333</v>
+        <v>41.01666666666668</v>
       </c>
       <c r="J18" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G18),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>1</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="3"/>
-        <v>33.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -7183,15 +7286,15 @@
       </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
-        <v>35.566666666666663</v>
+        <v>39.233333333333348</v>
       </c>
       <c r="J19" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G19),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>7</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="3"/>
-        <v>26.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -7221,15 +7324,15 @@
       </c>
       <c r="I20" s="8">
         <f t="shared" si="1"/>
-        <v>33.949999999999996</v>
+        <v>37.450000000000017</v>
       </c>
       <c r="J20" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G20),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>4</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -7259,15 +7362,15 @@
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
-        <v>32.333333333333329</v>
+        <v>35.666666666666686</v>
       </c>
       <c r="J21" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G21),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K21" s="8">
         <f>K20- J21</f>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -7297,15 +7400,15 @@
       </c>
       <c r="I22" s="8">
         <f t="shared" si="1"/>
-        <v>30.716666666666661</v>
+        <v>33.883333333333354</v>
       </c>
       <c r="J22" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G22),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -7335,15 +7438,15 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="1"/>
-        <v>29.099999999999994</v>
+        <v>32.100000000000023</v>
       </c>
       <c r="J23" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G23),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -7373,15 +7476,15 @@
       </c>
       <c r="I24" s="8">
         <f t="shared" si="1"/>
-        <v>27.483333333333327</v>
+        <v>30.316666666666688</v>
       </c>
       <c r="J24" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G24),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -7411,15 +7514,15 @@
       </c>
       <c r="I25" s="8">
         <f t="shared" si="1"/>
-        <v>25.86666666666666</v>
+        <v>28.533333333333353</v>
       </c>
       <c r="J25" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G25),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>2</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="3"/>
-        <v>20.5</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -7449,15 +7552,15 @@
       </c>
       <c r="I26" s="8">
         <f t="shared" si="1"/>
-        <v>24.249999999999993</v>
+        <v>26.750000000000018</v>
       </c>
       <c r="J26" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G26),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>4</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="3"/>
-        <v>16.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -7487,15 +7590,15 @@
       </c>
       <c r="I27" s="8">
         <f t="shared" si="1"/>
-        <v>22.633333333333326</v>
+        <v>24.966666666666683</v>
       </c>
       <c r="J27" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G27),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>1</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="3"/>
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -7525,15 +7628,15 @@
       </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
-        <v>21.016666666666659</v>
+        <v>23.183333333333348</v>
       </c>
       <c r="J28" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G28),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="3"/>
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -7563,15 +7666,15 @@
       </c>
       <c r="I29" s="8">
         <f t="shared" si="1"/>
-        <v>19.399999999999991</v>
+        <v>21.400000000000013</v>
       </c>
       <c r="J29" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G29),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K29" s="8">
         <f t="shared" si="3"/>
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -7601,15 +7704,15 @@
       </c>
       <c r="I30" s="8">
         <f t="shared" si="1"/>
-        <v>17.783333333333324</v>
+        <v>19.616666666666678</v>
       </c>
       <c r="J30" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G30),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K30" s="8">
         <f t="shared" si="3"/>
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -7639,15 +7742,15 @@
       </c>
       <c r="I31" s="8">
         <f t="shared" si="1"/>
-        <v>16.166666666666657</v>
+        <v>17.833333333333343</v>
       </c>
       <c r="J31" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G31),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>1.5</v>
       </c>
       <c r="K31" s="8">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -7677,15 +7780,15 @@
       </c>
       <c r="I32" s="8">
         <f t="shared" si="1"/>
-        <v>14.54999999999999</v>
+        <v>16.050000000000008</v>
       </c>
       <c r="J32" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G32),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>4</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -7715,15 +7818,15 @@
       </c>
       <c r="I33" s="8">
         <f t="shared" si="1"/>
-        <v>12.933333333333323</v>
+        <v>14.266666666666675</v>
       </c>
       <c r="J33" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G33),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -7753,15 +7856,15 @@
       </c>
       <c r="I34" s="8">
         <f t="shared" si="1"/>
-        <v>11.316666666666656</v>
+        <v>12.483333333333341</v>
       </c>
       <c r="J34" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G34),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -7791,15 +7894,15 @@
       </c>
       <c r="I35" s="8">
         <f t="shared" si="1"/>
-        <v>9.6999999999999886</v>
+        <v>10.700000000000008</v>
       </c>
       <c r="J35" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G35),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K35" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -7829,11 +7932,11 @@
       </c>
       <c r="I36" s="8">
         <f t="shared" si="1"/>
-        <v>8.0833333333333215</v>
+        <v>8.916666666666675</v>
       </c>
       <c r="J36" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B81)</f>
-        <v>0</v>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G36),'SPRINT-BACKLOG'!B40:B86)</f>
+        <v>5</v>
       </c>
       <c r="K36" s="8">
         <f t="shared" si="3"/>
@@ -7867,10 +7970,10 @@
       </c>
       <c r="I37" s="8">
         <f t="shared" si="1"/>
-        <v>6.4666666666666544</v>
+        <v>7.1333333333333417</v>
       </c>
       <c r="J37" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G37),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K37" s="8">
@@ -7905,10 +8008,10 @@
       </c>
       <c r="I38" s="8">
         <f t="shared" si="1"/>
-        <v>4.8499999999999872</v>
+        <v>5.3500000000000085</v>
       </c>
       <c r="J38" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G38),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K38" s="8">
@@ -7925,10 +8028,10 @@
       </c>
       <c r="I39" s="8">
         <f t="shared" si="1"/>
-        <v>3.2333333333333205</v>
+        <v>3.5666666666666753</v>
       </c>
       <c r="J39" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G39),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K39" s="8">
@@ -7945,10 +8048,10 @@
       </c>
       <c r="I40" s="8">
         <f t="shared" si="1"/>
-        <v>1.6166666666666538</v>
+        <v>1.7833333333333419</v>
       </c>
       <c r="J40" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G40),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K40" s="8">
@@ -7965,10 +8068,10 @@
       </c>
       <c r="I41" s="8">
         <f t="shared" si="1"/>
-        <v>-1.2878587085651816E-14</v>
+        <v>8.4376949871511897E-15</v>
       </c>
       <c r="J41" s="17">
-        <f>SUMIF('SPRINT-BACKLOG'!D40:D81,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B81)</f>
+        <f>SUMIF('SPRINT-BACKLOG'!D40:D86,"="&amp;VALUE(G41),'SPRINT-BACKLOG'!B40:B86)</f>
         <v>0</v>
       </c>
       <c r="K41" s="8">
@@ -7992,7 +8095,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>